<commit_message>
Add all fuctfunctions for `refGeo`
</commit_message>
<xml_diff>
--- a/Geo.xlsx
+++ b/Geo.xlsx
@@ -43,13 +43,13 @@
     <t>Executado</t>
   </si>
   <si>
-    <t>F03</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>71170</t>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>72752</t>
   </si>
 </sst>
 </file>
@@ -441,19 +441,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
-        <v>104</v>
+        <v>7375</v>
       </c>
       <c r="D2">
-        <v>570707</v>
+        <v>70740</v>
       </c>
       <c r="E2">
-        <v>7.07</v>
+        <v>0.7417</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Add read file function
</commit_message>
<xml_diff>
--- a/Geo.xlsx
+++ b/Geo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Location_i</t>
   </si>
@@ -38,30 +38,6 @@
   </si>
   <si>
     <t>poligono</t>
-  </si>
-  <si>
-    <t>Executado</t>
-  </si>
-  <si>
-    <t>F03</t>
-  </si>
-  <si>
-    <t>F02</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>41732</t>
-  </si>
-  <si>
-    <t>72752</t>
-  </si>
-  <si>
-    <t>12257</t>
   </si>
 </sst>
 </file>
@@ -419,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,84 +427,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>40140</v>
-      </c>
-      <c r="D2">
-        <v>41004.42</v>
-      </c>
-      <c r="E2">
-        <v>54.5455</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>7375</v>
-      </c>
-      <c r="D3">
-        <v>50000</v>
-      </c>
-      <c r="E3">
-        <v>0.7417</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>77575</v>
-      </c>
-      <c r="D4">
-        <v>752.0075000000001</v>
-      </c>
-      <c r="E4">
-        <v>752341</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>